<commit_message>
time scale update: s -> ms
</commit_message>
<xml_diff>
--- a/chart.xlsx
+++ b/chart.xlsx
@@ -293,7 +293,7 @@
               <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
               <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:r>
-                  <a:t>time elapsed (s)</a:t>
+                  <a:t>time elapsed (ms)</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -803,58 +803,58 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0004162827100694445</v>
+        <v>0.3126965</v>
       </c>
       <c r="D3" t="n">
-        <v>0.003191617532986111</v>
+        <v>3.195789401041667</v>
       </c>
       <c r="E3" t="n">
-        <v>0.003565061987847223</v>
+        <v>3.619022005208334</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004951618182291667</v>
+        <v>4.967390161458333</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00738425851388889</v>
+        <v>7.415865105902777</v>
       </c>
       <c r="H3" t="n">
-        <v>0.007624180805555557</v>
+        <v>7.655040432291666</v>
       </c>
       <c r="I3" t="n">
-        <v>0.008857244565972221</v>
+        <v>8.828057548611111</v>
       </c>
       <c r="J3" t="n">
-        <v>0.01105515652083333</v>
+        <v>11.02605521180556</v>
       </c>
       <c r="K3" t="n">
-        <v>0.013430735609375</v>
+        <v>13.35302809027778</v>
       </c>
       <c r="L3" t="n">
-        <v>0.01357188464756944</v>
+        <v>13.49793984895833</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01478801968055555</v>
+        <v>14.66949730555556</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01697507621354167</v>
+        <v>16.87689825694444</v>
       </c>
       <c r="O3" t="n">
-        <v>0.01927914072395833</v>
+        <v>19.20576161111111</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01935680719444444</v>
+        <v>19.28444795138888</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02124757717881945</v>
+        <v>21.15322092361111</v>
       </c>
       <c r="R3" t="n">
-        <v>0.02310120305729167</v>
+        <v>23.00321997222222</v>
       </c>
       <c r="S3" t="n">
-        <v>0.02490934516145833</v>
+        <v>24.80391318402777</v>
       </c>
       <c r="T3" t="n">
-        <v>0.02492662313020834</v>
+        <v>24.824139</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -1045,58 +1045,58 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0002241922482638888</v>
+        <v>0.1613542378472222</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0007647192621527778</v>
+        <v>0.7036061701388888</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0009272101909722223</v>
+        <v>0.8464881944444443</v>
       </c>
       <c r="F10" t="n">
-        <v>0.001214202609375</v>
+        <v>1.129266887152778</v>
       </c>
       <c r="G10" t="n">
-        <v>0.001715415170138889</v>
+        <v>1.618272729166667</v>
       </c>
       <c r="H10" t="n">
-        <v>0.001785800166666666</v>
+        <v>1.687166574652778</v>
       </c>
       <c r="I10" t="n">
-        <v>0.001953985388888889</v>
+        <v>1.867558008680556</v>
       </c>
       <c r="J10" t="n">
-        <v>0.002196694536458333</v>
+        <v>2.122761454861111</v>
       </c>
       <c r="K10" t="n">
-        <v>0.002412378138888888</v>
+        <v>2.329663388888889</v>
       </c>
       <c r="L10" t="n">
-        <v>0.002435857565972222</v>
+        <v>2.353591822916667</v>
       </c>
       <c r="M10" t="n">
-        <v>0.002531615805555556</v>
+        <v>2.439550385416667</v>
       </c>
       <c r="N10" t="n">
-        <v>0.002645469401041666</v>
+        <v>2.553520779513889</v>
       </c>
       <c r="O10" t="n">
-        <v>0.002755096770833333</v>
+        <v>2.649179206597222</v>
       </c>
       <c r="P10" t="n">
-        <v>0.002765018907986111</v>
+        <v>2.659316967013889</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.002846537708333333</v>
+        <v>2.737239118055555</v>
       </c>
       <c r="R10" t="n">
-        <v>0.002925650684027777</v>
+        <v>2.813186053819444</v>
       </c>
       <c r="S10" t="n">
-        <v>0.002999927585069444</v>
+        <v>2.887139371527779</v>
       </c>
       <c r="T10" t="n">
-        <v>0.003002142017361111</v>
+        <v>2.889305788194445</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1287,58 +1287,58 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0002656619652777778</v>
+        <v>0.1577050590277778</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0007685774305555555</v>
+        <v>0.6229637378472223</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0009047569027777777</v>
+        <v>0.7620447170138889</v>
       </c>
       <c r="F17" t="n">
-        <v>0.001177339413194444</v>
+        <v>0.9985711059027776</v>
       </c>
       <c r="G17" t="n">
-        <v>0.001629685324652778</v>
+        <v>1.429373045138889</v>
       </c>
       <c r="H17" t="n">
-        <v>0.001688005819444444</v>
+        <v>1.488095822916667</v>
       </c>
       <c r="I17" t="n">
-        <v>0.001845649479166667</v>
+        <v>1.640996751736111</v>
       </c>
       <c r="J17" t="n">
-        <v>0.002080251291666666</v>
+        <v>1.868069293402777</v>
       </c>
       <c r="K17" t="n">
-        <v>0.002272462694444444</v>
+        <v>2.054396899305555</v>
       </c>
       <c r="L17" t="n">
-        <v>0.002292781579861111</v>
+        <v>2.075141029513889</v>
       </c>
       <c r="M17" t="n">
-        <v>0.002374029642361111</v>
+        <v>2.156682425347222</v>
       </c>
       <c r="N17" t="n">
-        <v>0.002489335359375</v>
+        <v>2.263981713541667</v>
       </c>
       <c r="O17" t="n">
-        <v>0.002585660418402778</v>
+        <v>2.3581944375</v>
       </c>
       <c r="P17" t="n">
-        <v>0.002594568975694444</v>
+        <v>2.367740720486111</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.002669612428819444</v>
+        <v>2.440125642361112</v>
       </c>
       <c r="R17" t="n">
-        <v>0.002744115421875</v>
+        <v>2.5139573125</v>
       </c>
       <c r="S17" t="n">
-        <v>0.002814459696180556</v>
+        <v>2.580146041666667</v>
       </c>
       <c r="T17" t="n">
-        <v>0.002816312352430555</v>
+        <v>2.582103788194444</v>
       </c>
     </row>
     <row r="18" spans="1:20">

</xml_diff>